<commit_message>
Structuring and uploading thesis-relevant scripts
</commit_message>
<xml_diff>
--- a/Parameters/demand_parameters.xlsx
+++ b/Parameters/demand_parameters.xlsx
@@ -425,7 +425,7 @@
     <col min="5" max="5" style="6" width="29.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -453,41 +453,41 @@
         <v>102.63</v>
       </c>
       <c r="D2" s="5">
-        <v>7411300</v>
+        <v>6492300</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="1"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>

</xml_diff>